<commit_message>
new R values for analysis
</commit_message>
<xml_diff>
--- a/models/projections.xlsx
+++ b/models/projections.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid-litsearch/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD56ABCF-8905-7F48-ADE7-B3B70D9B042D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A2FD73-DA71-0A41-AF11-3E3CBE6810C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{C18A3728-632D-6949-A56C-88ED3B6942BE}"/>
+    <workbookView xWindow="20480" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{C18A3728-632D-6949-A56C-88ED3B6942BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="simulations" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$T$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$T$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="52">
   <si>
     <t>First confirmed case</t>
   </si>
@@ -172,13 +172,34 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Can't introduce virus early enough to match death date here - should be November</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +230,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -243,6 +271,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,18 +588,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274A361D-3095-2A4A-BF18-56AC773A1DCE}">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="6.5" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
@@ -1371,11 +1404,11 @@
         <v>2.4</v>
       </c>
       <c r="F15" s="7">
-        <f>F3-G15</f>
+        <f t="shared" ref="F15:F27" si="0">F3-G15</f>
         <v>43841</v>
       </c>
       <c r="G15" s="8">
-        <f>I3-C3</f>
+        <f t="shared" ref="G15:G26" si="1">I3-C3</f>
         <v>2</v>
       </c>
       <c r="H15" s="6">
@@ -1435,11 +1468,11 @@
         <v>2.4</v>
       </c>
       <c r="F16" s="7">
-        <f>F4-G16</f>
+        <f t="shared" si="0"/>
         <v>43839</v>
       </c>
       <c r="G16" s="8">
-        <f>I4-C4</f>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="H16" s="6">
@@ -1499,11 +1532,11 @@
         <v>2.4</v>
       </c>
       <c r="F17" s="7">
-        <f>F5-G17</f>
+        <f t="shared" si="0"/>
         <v>43821</v>
       </c>
       <c r="G17" s="8">
-        <f>I5-C5</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H17" s="6">
@@ -1563,11 +1596,11 @@
         <v>2.4</v>
       </c>
       <c r="F18" s="7">
-        <f>F6-G18</f>
+        <f t="shared" si="0"/>
         <v>43816</v>
       </c>
       <c r="G18" s="8">
-        <f>I6-C6</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="H18" s="6">
@@ -1627,11 +1660,11 @@
         <v>2.4</v>
       </c>
       <c r="F19" s="7">
-        <f>F7-G19</f>
+        <f t="shared" si="0"/>
         <v>43842</v>
       </c>
       <c r="G19" s="8">
-        <f>I7-C7</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H19" s="6">
@@ -1691,11 +1724,11 @@
         <v>2.4</v>
       </c>
       <c r="F20" s="7">
-        <f>F8-G20</f>
+        <f t="shared" si="0"/>
         <v>43837</v>
       </c>
       <c r="G20" s="8">
-        <f>I8-C8</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="H20" s="6">
@@ -1755,11 +1788,11 @@
         <v>1.9</v>
       </c>
       <c r="F21" s="2">
-        <f>F9-G21</f>
+        <f t="shared" si="0"/>
         <v>43828</v>
       </c>
       <c r="G21" s="5">
-        <f>I9-C9</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H21">
@@ -1819,11 +1852,11 @@
         <v>1.8</v>
       </c>
       <c r="F22" s="2">
-        <f>F10-G22</f>
+        <f t="shared" si="0"/>
         <v>43819</v>
       </c>
       <c r="G22" s="5">
-        <f>I10-C10</f>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="H22">
@@ -1881,11 +1914,11 @@
         <v>1.8</v>
       </c>
       <c r="F23" s="7">
-        <f>F11-G23</f>
+        <f t="shared" si="0"/>
         <v>43803</v>
       </c>
       <c r="G23" s="8">
-        <f>I11-C11</f>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="H23" s="6">
@@ -1945,11 +1978,11 @@
         <v>2</v>
       </c>
       <c r="F24" s="2">
-        <f>F12-G24</f>
+        <f t="shared" si="0"/>
         <v>43806</v>
       </c>
       <c r="G24" s="5">
-        <f>I12-C12</f>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="H24">
@@ -2009,11 +2042,11 @@
         <v>1.8</v>
       </c>
       <c r="F25" s="2">
-        <f>F13-G25</f>
+        <f t="shared" si="0"/>
         <v>43824</v>
       </c>
       <c r="G25" s="5">
-        <f>I13-C13</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="H25">
@@ -2073,11 +2106,11 @@
         <v>1.9</v>
       </c>
       <c r="F26" s="2">
-        <f>F14-G26</f>
+        <f t="shared" si="0"/>
         <v>43824</v>
       </c>
       <c r="G26" s="5">
-        <f>I14-C14</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="H26">
@@ -2137,7 +2170,7 @@
         <v>2.6</v>
       </c>
       <c r="F27" s="7">
-        <f>F15-G27</f>
+        <f t="shared" si="0"/>
         <v>43841</v>
       </c>
       <c r="I27" s="7">
@@ -2529,11 +2562,11 @@
         <v>2.6</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" ref="F38:F46" si="0">F28-G38</f>
+        <f t="shared" ref="F38:F48" si="2">F28-G38</f>
         <v>43842</v>
       </c>
       <c r="G38">
-        <f t="shared" ref="G38:G46" si="1">I28-C28</f>
+        <f t="shared" ref="G38:G46" si="3">I28-C28</f>
         <v>34</v>
       </c>
       <c r="I38" s="2">
@@ -2746,11 +2779,11 @@
         <v>3.8</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43853</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-12</v>
       </c>
       <c r="I42" s="2">
@@ -2804,11 +2837,11 @@
         <v>3.8</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43853</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="I43" s="2">
@@ -2862,11 +2895,11 @@
         <v>3.8</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43828</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-12</v>
       </c>
       <c r="I44" s="2">
@@ -2920,11 +2953,11 @@
         <v>3.8</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43855</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-13</v>
       </c>
       <c r="I45" s="2">
@@ -2978,11 +3011,11 @@
         <v>3.8</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43850</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-13</v>
       </c>
       <c r="I46" s="2">
@@ -3017,6 +3050,1673 @@
       </c>
       <c r="T46" s="5">
         <v>204775.82915687899</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="7">
+        <v>43857</v>
+      </c>
+      <c r="C47" s="7">
+        <v>43899</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E47" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F47" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I47" s="7">
+        <v>43916</v>
+      </c>
+      <c r="K47" s="8">
+        <v>34762001.723133802</v>
+      </c>
+      <c r="L47" s="8">
+        <v>12461343.346810499</v>
+      </c>
+      <c r="M47" s="8">
+        <v>23407996.155429401</v>
+      </c>
+      <c r="N47" s="8">
+        <v>502362.188761884</v>
+      </c>
+      <c r="O47" s="8">
+        <v>466.97819722632102</v>
+      </c>
+      <c r="P47" s="8">
+        <v>3905.8977171773599</v>
+      </c>
+      <c r="Q47" s="8">
+        <v>10880.5793563111</v>
+      </c>
+      <c r="R47" s="8">
+        <v>54151.3395547541</v>
+      </c>
+      <c r="S47" s="8">
+        <v>205059.13536340301</v>
+      </c>
+      <c r="T47" s="8">
+        <v>227898.25857301199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C48" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E48" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F48" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I48" s="7">
+        <v>43920</v>
+      </c>
+      <c r="K48" s="8">
+        <v>1938817.5824211501</v>
+      </c>
+      <c r="L48" s="8">
+        <v>484627.87075805099</v>
+      </c>
+      <c r="M48" s="8">
+        <v>910176.01478709397</v>
+      </c>
+      <c r="N48" s="8">
+        <v>19595.502925072102</v>
+      </c>
+      <c r="O48" s="8">
+        <v>64.478710113177897</v>
+      </c>
+      <c r="P48" s="8">
+        <v>251.417104322466</v>
+      </c>
+      <c r="Q48" s="8">
+        <v>778.94872879239301</v>
+      </c>
+      <c r="R48" s="8">
+        <v>2525.7977576651501</v>
+      </c>
+      <c r="S48" s="8">
+        <v>9137.9094328558404</v>
+      </c>
+      <c r="T48" s="8">
+        <v>6836.9511913230599</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C49" s="7">
+        <v>43874</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E49" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F49" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I49" s="7">
+        <v>43916</v>
+      </c>
+      <c r="K49" s="8">
+        <v>19437270.282523599</v>
+      </c>
+      <c r="L49" s="8">
+        <v>6982842.3662573602</v>
+      </c>
+      <c r="M49" s="8">
+        <v>13116241.6123896</v>
+      </c>
+      <c r="N49" s="8">
+        <v>281771.83058807102</v>
+      </c>
+      <c r="O49" s="8">
+        <v>301.03136752367402</v>
+      </c>
+      <c r="P49" s="8">
+        <v>1862.43984759157</v>
+      </c>
+      <c r="Q49" s="8">
+        <v>7308.6547161550297</v>
+      </c>
+      <c r="R49" s="8">
+        <v>29195.457692570999</v>
+      </c>
+      <c r="S49" s="8">
+        <v>104901.375260175</v>
+      </c>
+      <c r="T49" s="8">
+        <v>138202.87170405401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C50" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F50" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I50" s="7">
+        <v>43917</v>
+      </c>
+      <c r="K50" s="8">
+        <v>4099520.7423055498</v>
+      </c>
+      <c r="L50" s="8">
+        <v>1406708.96086898</v>
+      </c>
+      <c r="M50" s="8">
+        <v>2641963.1106505799</v>
+      </c>
+      <c r="N50" s="8">
+        <v>56868.477823284702</v>
+      </c>
+      <c r="O50" s="8">
+        <v>72.900927213856704</v>
+      </c>
+      <c r="P50" s="8">
+        <v>533.49247745021</v>
+      </c>
+      <c r="Q50" s="8">
+        <v>1315.23940880546</v>
+      </c>
+      <c r="R50" s="8">
+        <v>5501.5057355224699</v>
+      </c>
+      <c r="S50" s="8">
+        <v>25563.319091483001</v>
+      </c>
+      <c r="T50" s="8">
+        <v>23882.020182809702</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C51" s="7">
+        <v>43895</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" s="6">
+        <v>2.7</v>
+      </c>
+      <c r="F51" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I51" s="7">
+        <v>43916</v>
+      </c>
+      <c r="K51" s="8">
+        <v>29296391.548263099</v>
+      </c>
+      <c r="L51" s="8">
+        <v>9662298.29288112</v>
+      </c>
+      <c r="M51" s="8">
+        <v>18148246.798771001</v>
+      </c>
+      <c r="N51" s="8">
+        <v>390121.42114917201</v>
+      </c>
+      <c r="O51" s="8">
+        <v>769.40504801423197</v>
+      </c>
+      <c r="P51" s="8">
+        <v>3702.90955030447</v>
+      </c>
+      <c r="Q51" s="8">
+        <v>9417.6348847929094</v>
+      </c>
+      <c r="R51" s="8">
+        <v>37738.760668876101</v>
+      </c>
+      <c r="S51" s="8">
+        <v>169498.83091003899</v>
+      </c>
+      <c r="T51" s="8">
+        <v>168993.88008714499</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="7">
+        <v>43857</v>
+      </c>
+      <c r="C52" s="7">
+        <v>43899</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F52" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I52" s="7">
+        <v>43951</v>
+      </c>
+      <c r="K52" s="8">
+        <v>836881.661514343</v>
+      </c>
+      <c r="L52" s="8">
+        <v>93679.828297261905</v>
+      </c>
+      <c r="M52" s="8">
+        <v>186723.25925658201</v>
+      </c>
+      <c r="N52" s="8">
+        <v>2069.1882433259898</v>
+      </c>
+      <c r="O52" s="8">
+        <v>1.2980422958389699</v>
+      </c>
+      <c r="P52" s="8">
+        <v>23.1334879012561</v>
+      </c>
+      <c r="Q52" s="8">
+        <v>81.390779914524998</v>
+      </c>
+      <c r="R52" s="8">
+        <v>372.65219345870599</v>
+      </c>
+      <c r="S52" s="8">
+        <v>826.988530797257</v>
+      </c>
+      <c r="T52" s="8">
+        <v>763.72520895840398</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C53" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F53" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I53" s="7">
+        <v>43959</v>
+      </c>
+      <c r="K53" s="8">
+        <v>451564.46602952102</v>
+      </c>
+      <c r="L53" s="8">
+        <v>44310.574880207103</v>
+      </c>
+      <c r="M53" s="8">
+        <v>87605.011303009494</v>
+      </c>
+      <c r="N53" s="8">
+        <v>1061.3719295062999</v>
+      </c>
+      <c r="O53" s="8">
+        <v>2.5694211146075201</v>
+      </c>
+      <c r="P53" s="8">
+        <v>19.384526011228001</v>
+      </c>
+      <c r="Q53" s="8">
+        <v>78.965672106698406</v>
+      </c>
+      <c r="R53" s="8">
+        <v>203.39778479562199</v>
+      </c>
+      <c r="S53" s="8">
+        <v>474.10286798066801</v>
+      </c>
+      <c r="T53" s="8">
+        <v>282.95165749747702</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C54" s="7">
+        <v>43874</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F54" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I54" s="7">
+        <v>43951</v>
+      </c>
+      <c r="K54" s="8">
+        <v>781947.60358773905</v>
+      </c>
+      <c r="L54" s="8">
+        <v>90244.069692586301</v>
+      </c>
+      <c r="M54" s="8">
+        <v>179783.92944727099</v>
+      </c>
+      <c r="N54" s="8">
+        <v>2003.4193731775399</v>
+      </c>
+      <c r="O54" s="8">
+        <v>1.29810862171741</v>
+      </c>
+      <c r="P54" s="8">
+        <v>17.994526297029601</v>
+      </c>
+      <c r="Q54" s="8">
+        <v>98.917810156540696</v>
+      </c>
+      <c r="R54" s="8">
+        <v>308.60594642772998</v>
+      </c>
+      <c r="S54" s="8">
+        <v>724.89243864207401</v>
+      </c>
+      <c r="T54" s="8">
+        <v>851.71054303244603</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C55" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F55" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I55" s="7">
+        <v>43952</v>
+      </c>
+      <c r="K55" s="8">
+        <v>624526.26279988897</v>
+      </c>
+      <c r="L55" s="8">
+        <v>77427.901272685995</v>
+      </c>
+      <c r="M55" s="8">
+        <v>153663.92759988099</v>
+      </c>
+      <c r="N55" s="8">
+        <v>1785.58057303889</v>
+      </c>
+      <c r="O55" s="8">
+        <v>1.36429914003193</v>
+      </c>
+      <c r="P55" s="8">
+        <v>23.557558583310801</v>
+      </c>
+      <c r="Q55" s="8">
+        <v>73.453431767786796</v>
+      </c>
+      <c r="R55" s="8">
+        <v>286.35810680343798</v>
+      </c>
+      <c r="S55" s="8">
+        <v>823.48541758362205</v>
+      </c>
+      <c r="T55" s="8">
+        <v>577.36175916069703</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C56" s="7">
+        <v>43895</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F56" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I56" s="7">
+        <v>43951</v>
+      </c>
+      <c r="K56" s="8">
+        <v>872515.97148953495</v>
+      </c>
+      <c r="L56" s="8">
+        <v>97231.489666640904</v>
+      </c>
+      <c r="M56" s="8">
+        <v>193782.09531221201</v>
+      </c>
+      <c r="N56" s="8">
+        <v>2149.7797831906</v>
+      </c>
+      <c r="O56" s="8">
+        <v>3.7217041221254199</v>
+      </c>
+      <c r="P56" s="8">
+        <v>27.469307609379499</v>
+      </c>
+      <c r="Q56" s="8">
+        <v>86.429911481632999</v>
+      </c>
+      <c r="R56" s="8">
+        <v>281.17923372926299</v>
+      </c>
+      <c r="S56" s="8">
+        <v>1006.64723774043</v>
+      </c>
+      <c r="T56" s="8">
+        <v>744.33238850777502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="7">
+        <v>43857</v>
+      </c>
+      <c r="C57" s="7">
+        <v>43899</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E57" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F57" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I57" s="7">
+        <v>43907</v>
+      </c>
+      <c r="K57" s="8">
+        <v>39533443.041606799</v>
+      </c>
+      <c r="L57" s="8">
+        <v>15227648.959415499</v>
+      </c>
+      <c r="M57" s="8">
+        <v>28598269.924647599</v>
+      </c>
+      <c r="N57" s="8">
+        <v>615929.19489634701</v>
+      </c>
+      <c r="O57" s="8">
+        <v>647.72050272705701</v>
+      </c>
+      <c r="P57" s="8">
+        <v>4298.5171089984897</v>
+      </c>
+      <c r="Q57" s="8">
+        <v>11401.4131864717</v>
+      </c>
+      <c r="R57" s="8">
+        <v>57932.845015864797</v>
+      </c>
+      <c r="S57" s="8">
+        <v>240819.07073916201</v>
+      </c>
+      <c r="T57" s="8">
+        <v>300829.62834312301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C58" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F58" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I58" s="7">
+        <v>43910</v>
+      </c>
+      <c r="K58" s="8">
+        <v>2193082.94771781</v>
+      </c>
+      <c r="L58" s="8">
+        <v>589686.88687779906</v>
+      </c>
+      <c r="M58" s="8">
+        <v>1107460.7493447999</v>
+      </c>
+      <c r="N58" s="8">
+        <v>23851.721223914101</v>
+      </c>
+      <c r="O58" s="8">
+        <v>77.7294776994773</v>
+      </c>
+      <c r="P58" s="8">
+        <v>275.558638920345</v>
+      </c>
+      <c r="Q58" s="8">
+        <v>813.01793869995697</v>
+      </c>
+      <c r="R58" s="8">
+        <v>2730.3416418669899</v>
+      </c>
+      <c r="S58" s="8">
+        <v>11030.315925818</v>
+      </c>
+      <c r="T58" s="8">
+        <v>8924.7576009093991</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C59" s="7">
+        <v>43874</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E59" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F59" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I59" s="7">
+        <v>43907</v>
+      </c>
+      <c r="K59" s="8">
+        <v>22152798.165196601</v>
+      </c>
+      <c r="L59" s="8">
+        <v>8401247.2611769605</v>
+      </c>
+      <c r="M59" s="8">
+        <v>15777956.312563799</v>
+      </c>
+      <c r="N59" s="8">
+        <v>339813.41876861698</v>
+      </c>
+      <c r="O59" s="8">
+        <v>431.50462031304897</v>
+      </c>
+      <c r="P59" s="8">
+        <v>2101.9733207814102</v>
+      </c>
+      <c r="Q59" s="8">
+        <v>7645.3692984956597</v>
+      </c>
+      <c r="R59" s="8">
+        <v>31629.680335962199</v>
+      </c>
+      <c r="S59" s="8">
+        <v>125841.5818979</v>
+      </c>
+      <c r="T59" s="8">
+        <v>172163.30929516401</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C60" s="7">
+        <v>43901</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E60" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F60" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I60" s="7">
+        <v>43907</v>
+      </c>
+      <c r="K60" s="8">
+        <v>4644718.5795150902</v>
+      </c>
+      <c r="L60" s="8">
+        <v>1691688.0874347501</v>
+      </c>
+      <c r="M60" s="8">
+        <v>3177072.95250188</v>
+      </c>
+      <c r="N60" s="8">
+        <v>68425.565906317002</v>
+      </c>
+      <c r="O60" s="8">
+        <v>102.44343408125501</v>
+      </c>
+      <c r="P60" s="8">
+        <v>583.59980332563998</v>
+      </c>
+      <c r="Q60" s="8">
+        <v>1377.6499648573399</v>
+      </c>
+      <c r="R60" s="8">
+        <v>5809.3998607886897</v>
+      </c>
+      <c r="S60" s="8">
+        <v>29715.418680085499</v>
+      </c>
+      <c r="T60" s="8">
+        <v>30837.054163178502</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="7">
+        <v>43861</v>
+      </c>
+      <c r="C61" s="7">
+        <v>43895</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E61" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F61" s="7">
+        <v>43862</v>
+      </c>
+      <c r="I61" s="7">
+        <v>43907</v>
+      </c>
+      <c r="K61" s="8">
+        <v>32247215.251966</v>
+      </c>
+      <c r="L61" s="8">
+        <v>11203461.262452399</v>
+      </c>
+      <c r="M61" s="8">
+        <v>21040646.956838202</v>
+      </c>
+      <c r="N61" s="8">
+        <v>453159.03646266903</v>
+      </c>
+      <c r="O61" s="8">
+        <v>886.97071338683099</v>
+      </c>
+      <c r="P61" s="8">
+        <v>3977.14462195738</v>
+      </c>
+      <c r="Q61" s="8">
+        <v>9759.0938164898107</v>
+      </c>
+      <c r="R61" s="8">
+        <v>40406.749166830799</v>
+      </c>
+      <c r="S61" s="8">
+        <v>191217.491365144</v>
+      </c>
+      <c r="T61" s="8">
+        <v>206911.58677885999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="2">
+        <v>43857</v>
+      </c>
+      <c r="C62" s="2">
+        <v>43899</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62">
+        <v>2.7</v>
+      </c>
+      <c r="F62" s="2">
+        <f>F47-G62</f>
+        <v>43845</v>
+      </c>
+      <c r="G62">
+        <f>I47-C47</f>
+        <v>17</v>
+      </c>
+      <c r="I62" s="2">
+        <v>43899</v>
+      </c>
+      <c r="K62" s="5">
+        <v>34764562.636573002</v>
+      </c>
+      <c r="L62" s="5">
+        <v>12474479.7878277</v>
+      </c>
+      <c r="M62" s="5">
+        <v>23428053.9930069</v>
+      </c>
+      <c r="N62" s="5">
+        <v>504444.57797109801</v>
+      </c>
+      <c r="O62" s="5">
+        <v>471.03820035430198</v>
+      </c>
+      <c r="P62" s="5">
+        <v>3914.4558045853701</v>
+      </c>
+      <c r="Q62" s="5">
+        <v>10894.1605412238</v>
+      </c>
+      <c r="R62" s="5">
+        <v>54226.883106569701</v>
+      </c>
+      <c r="S62" s="5">
+        <v>205838.961706712</v>
+      </c>
+      <c r="T62" s="5">
+        <v>229099.07861165199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="2">
+        <v>43890</v>
+      </c>
+      <c r="C63" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63">
+        <v>2.7</v>
+      </c>
+      <c r="F63" s="2">
+        <f t="shared" ref="F63:F76" si="4">F48-G63</f>
+        <v>43843</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ref="G63:G76" si="5">I48-C48</f>
+        <v>19</v>
+      </c>
+      <c r="I63" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K63" s="5">
+        <v>1938838.3052718199</v>
+      </c>
+      <c r="L63" s="5">
+        <v>484689.89548975899</v>
+      </c>
+      <c r="M63" s="5">
+        <v>910272.74576320394</v>
+      </c>
+      <c r="N63" s="5">
+        <v>19604.324294009399</v>
+      </c>
+      <c r="O63" s="5">
+        <v>64.530852023260394</v>
+      </c>
+      <c r="P63" s="5">
+        <v>251.47585183582001</v>
+      </c>
+      <c r="Q63" s="5">
+        <v>779.03017653178802</v>
+      </c>
+      <c r="R63" s="5">
+        <v>2526.2150762859101</v>
+      </c>
+      <c r="S63" s="5">
+        <v>9141.8377323364093</v>
+      </c>
+      <c r="T63" s="5">
+        <v>6841.2346049962598</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C64" s="2">
+        <v>43874</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64">
+        <v>2.7</v>
+      </c>
+      <c r="F64" s="2">
+        <f t="shared" si="4"/>
+        <v>43820</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="I64" s="2">
+        <v>43874</v>
+      </c>
+      <c r="K64" s="5">
+        <v>19439205.858956601</v>
+      </c>
+      <c r="L64" s="5">
+        <v>6989723.7694481397</v>
+      </c>
+      <c r="M64" s="5">
+        <v>13127049.7186793</v>
+      </c>
+      <c r="N64" s="5">
+        <v>282719.07017175702</v>
+      </c>
+      <c r="O64" s="5">
+        <v>304.08821354993898</v>
+      </c>
+      <c r="P64" s="5">
+        <v>1866.7299426525699</v>
+      </c>
+      <c r="Q64" s="5">
+        <v>7315.1615233640096</v>
+      </c>
+      <c r="R64" s="5">
+        <v>29239.612392237399</v>
+      </c>
+      <c r="S64" s="5">
+        <v>105236.417800134</v>
+      </c>
+      <c r="T64" s="5">
+        <v>138757.06029981899</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C65" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E65">
+        <v>2.7</v>
+      </c>
+      <c r="F65" s="2">
+        <f t="shared" si="4"/>
+        <v>43846</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="I65" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K65" s="5">
+        <v>4099594.2522574998</v>
+      </c>
+      <c r="L65" s="5">
+        <v>1406978.2971218301</v>
+      </c>
+      <c r="M65" s="5">
+        <v>2642384.2308579301</v>
+      </c>
+      <c r="N65" s="5">
+        <v>56906.395138805099</v>
+      </c>
+      <c r="O65" s="5">
+        <v>73.059259787751998</v>
+      </c>
+      <c r="P65" s="5">
+        <v>533.68009640406797</v>
+      </c>
+      <c r="Q65" s="5">
+        <v>1315.4712364273601</v>
+      </c>
+      <c r="R65" s="5">
+        <v>5502.6349122621104</v>
+      </c>
+      <c r="S65" s="5">
+        <v>25577.301395682</v>
+      </c>
+      <c r="T65" s="5">
+        <v>23904.248238241798</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C66" s="2">
+        <v>43895</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66">
+        <v>2.7</v>
+      </c>
+      <c r="F66" s="2">
+        <f t="shared" si="4"/>
+        <v>43841</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="I66" s="2">
+        <v>43895</v>
+      </c>
+      <c r="K66" s="5">
+        <v>29297252.0242466</v>
+      </c>
+      <c r="L66" s="5">
+        <v>9667315.6295820307</v>
+      </c>
+      <c r="M66" s="5">
+        <v>18155753.235848401</v>
+      </c>
+      <c r="N66" s="5">
+        <v>391002.60664248001</v>
+      </c>
+      <c r="O66" s="5">
+        <v>771.57044169642802</v>
+      </c>
+      <c r="P66" s="5">
+        <v>3707.3560386623899</v>
+      </c>
+      <c r="Q66" s="5">
+        <v>9424.2314716164201</v>
+      </c>
+      <c r="R66" s="5">
+        <v>37780.923177845798</v>
+      </c>
+      <c r="S66" s="5">
+        <v>169819.43355622701</v>
+      </c>
+      <c r="T66" s="5">
+        <v>169499.09195643201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="2">
+        <v>43857</v>
+      </c>
+      <c r="C67" s="2">
+        <v>43899</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67">
+        <v>1.6</v>
+      </c>
+      <c r="F67" s="2">
+        <f t="shared" si="4"/>
+        <v>43810</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="I67" s="2">
+        <v>43899</v>
+      </c>
+      <c r="K67" s="5">
+        <v>13015023.5384517</v>
+      </c>
+      <c r="L67" s="5">
+        <v>2246050.4416561699</v>
+      </c>
+      <c r="M67" s="5">
+        <v>4403206.7424908197</v>
+      </c>
+      <c r="N67" s="5">
+        <v>58509.488712165497</v>
+      </c>
+      <c r="O67" s="5">
+        <v>38.076027771864503</v>
+      </c>
+      <c r="P67" s="5">
+        <v>632.16351641376696</v>
+      </c>
+      <c r="Q67" s="5">
+        <v>2164.4588513824401</v>
+      </c>
+      <c r="R67" s="5">
+        <v>10009.8705541772</v>
+      </c>
+      <c r="S67" s="5">
+        <v>23624.318745749501</v>
+      </c>
+      <c r="T67" s="5">
+        <v>22040.601016670698</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="2">
+        <v>43890</v>
+      </c>
+      <c r="C68" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68">
+        <v>1.6</v>
+      </c>
+      <c r="F68" s="2">
+        <f t="shared" si="4"/>
+        <v>43804</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="5"/>
+        <v>58</v>
+      </c>
+      <c r="I68" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K68" s="5">
+        <v>1174783.83132131</v>
+      </c>
+      <c r="L68" s="5">
+        <v>237521.59541671799</v>
+      </c>
+      <c r="M68" s="5">
+        <v>449041.20725982601</v>
+      </c>
+      <c r="N68" s="5">
+        <v>8941.5966006357594</v>
+      </c>
+      <c r="O68" s="5">
+        <v>25.4124914227001</v>
+      </c>
+      <c r="P68" s="5">
+        <v>142.80846727274499</v>
+      </c>
+      <c r="Q68" s="5">
+        <v>516.235520987124</v>
+      </c>
+      <c r="R68" s="5">
+        <v>1483.6703678475899</v>
+      </c>
+      <c r="S68" s="5">
+        <v>4112.1373858102797</v>
+      </c>
+      <c r="T68" s="5">
+        <v>2661.3323672953202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="13">
+        <v>43861</v>
+      </c>
+      <c r="C69" s="13">
+        <v>43874</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="F69" s="13">
+        <v>44166</v>
+      </c>
+      <c r="G69" s="12">
+        <f t="shared" si="5"/>
+        <v>77</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I69" s="13">
+        <v>43889</v>
+      </c>
+      <c r="K69" s="14">
+        <v>10068073.2472206</v>
+      </c>
+      <c r="L69" s="14">
+        <v>2368734.3285799501</v>
+      </c>
+      <c r="M69" s="14">
+        <v>4564394.8126493096</v>
+      </c>
+      <c r="N69" s="14">
+        <v>73268.623655713498</v>
+      </c>
+      <c r="O69" s="14">
+        <v>52.029889656208702</v>
+      </c>
+      <c r="P69" s="14">
+        <v>611.71117940815202</v>
+      </c>
+      <c r="Q69" s="14">
+        <v>3090.00672535697</v>
+      </c>
+      <c r="R69" s="14">
+        <v>10357.812488576399</v>
+      </c>
+      <c r="S69" s="14">
+        <v>26848.096805214798</v>
+      </c>
+      <c r="T69" s="14">
+        <v>32308.966567501</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C70" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E70">
+        <v>1.6</v>
+      </c>
+      <c r="F70" s="2">
+        <f t="shared" si="4"/>
+        <v>43811</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="5"/>
+        <v>51</v>
+      </c>
+      <c r="I70" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K70" s="5">
+        <v>2382931.5266845101</v>
+      </c>
+      <c r="L70" s="5">
+        <v>606825.16572773003</v>
+      </c>
+      <c r="M70" s="5">
+        <v>1157883.9028744199</v>
+      </c>
+      <c r="N70" s="5">
+        <v>20734.4104706689</v>
+      </c>
+      <c r="O70" s="5">
+        <v>18.1368459124315</v>
+      </c>
+      <c r="P70" s="5">
+        <v>247.39930469009801</v>
+      </c>
+      <c r="Q70" s="5">
+        <v>712.12346742421596</v>
+      </c>
+      <c r="R70" s="5">
+        <v>2856.0923468114702</v>
+      </c>
+      <c r="S70" s="5">
+        <v>9628.84287129519</v>
+      </c>
+      <c r="T70" s="5">
+        <v>7271.8156345355201</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>13</v>
+      </c>
+      <c r="B71" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C71" s="2">
+        <v>43895</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E71">
+        <v>1.6</v>
+      </c>
+      <c r="F71" s="2">
+        <f t="shared" si="4"/>
+        <v>43806</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="5"/>
+        <v>56</v>
+      </c>
+      <c r="I71" s="2">
+        <v>43895</v>
+      </c>
+      <c r="K71" s="5">
+        <v>13670016.913458699</v>
+      </c>
+      <c r="L71" s="5">
+        <v>2567252.29134838</v>
+      </c>
+      <c r="M71" s="5">
+        <v>5002211.7976352004</v>
+      </c>
+      <c r="N71" s="5">
+        <v>71044.722394027805</v>
+      </c>
+      <c r="O71" s="5">
+        <v>126.32015832058801</v>
+      </c>
+      <c r="P71" s="5">
+        <v>871.49729038049395</v>
+      </c>
+      <c r="Q71" s="5">
+        <v>2648.9491038800702</v>
+      </c>
+      <c r="R71" s="5">
+        <v>8926.7929778276703</v>
+      </c>
+      <c r="S71" s="5">
+        <v>33015.582111644399</v>
+      </c>
+      <c r="T71" s="5">
+        <v>25455.580751974601</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="2">
+        <v>43857</v>
+      </c>
+      <c r="C72" s="2">
+        <v>43899</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E72">
+        <v>3.9</v>
+      </c>
+      <c r="F72" s="2">
+        <f t="shared" si="4"/>
+        <v>43854</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="I72" s="2">
+        <v>43899</v>
+      </c>
+      <c r="K72" s="5">
+        <v>39533443.425565802</v>
+      </c>
+      <c r="L72" s="5">
+        <v>15227652.948998099</v>
+      </c>
+      <c r="M72" s="5">
+        <v>28598275.543589901</v>
+      </c>
+      <c r="N72" s="5">
+        <v>615930.14005309797</v>
+      </c>
+      <c r="O72" s="5">
+        <v>647.72581162581002</v>
+      </c>
+      <c r="P72" s="5">
+        <v>4298.52029857257</v>
+      </c>
+      <c r="Q72" s="5">
+        <v>11401.416133463101</v>
+      </c>
+      <c r="R72" s="5">
+        <v>57932.858401000201</v>
+      </c>
+      <c r="S72" s="5">
+        <v>240819.28909310099</v>
+      </c>
+      <c r="T72" s="5">
+        <v>300830.33031533501</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="2">
+        <v>43890</v>
+      </c>
+      <c r="C73" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73">
+        <v>3.9</v>
+      </c>
+      <c r="F73" s="2">
+        <f t="shared" si="4"/>
+        <v>43853</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="I73" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K73" s="5">
+        <v>2193082.9496058798</v>
+      </c>
+      <c r="L73" s="5">
+        <v>589686.90538732905</v>
+      </c>
+      <c r="M73" s="5">
+        <v>1107460.7753085</v>
+      </c>
+      <c r="N73" s="5">
+        <v>23851.725654727299</v>
+      </c>
+      <c r="O73" s="5">
+        <v>77.729499401791898</v>
+      </c>
+      <c r="P73" s="5">
+        <v>275.5586543631</v>
+      </c>
+      <c r="Q73" s="5">
+        <v>813.01795187266498</v>
+      </c>
+      <c r="R73" s="5">
+        <v>2730.34173263412</v>
+      </c>
+      <c r="S73" s="5">
+        <v>11030.3176889186</v>
+      </c>
+      <c r="T73" s="5">
+        <v>8924.7601275369998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C74" s="2">
+        <v>43874</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74">
+        <v>3.9</v>
+      </c>
+      <c r="F74" s="2">
+        <f t="shared" si="4"/>
+        <v>43829</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="I74" s="2">
+        <v>43874</v>
+      </c>
+      <c r="K74" s="5">
+        <v>22152800.301895</v>
+      </c>
+      <c r="L74" s="5">
+        <v>8401258.1522349603</v>
+      </c>
+      <c r="M74" s="5">
+        <v>15777972.646609901</v>
+      </c>
+      <c r="N74" s="5">
+        <v>339815.31454400101</v>
+      </c>
+      <c r="O74" s="5">
+        <v>431.51934111368701</v>
+      </c>
+      <c r="P74" s="5">
+        <v>2101.9819414948902</v>
+      </c>
+      <c r="Q74" s="5">
+        <v>7645.3748094628399</v>
+      </c>
+      <c r="R74" s="5">
+        <v>31629.730770377399</v>
+      </c>
+      <c r="S74" s="5">
+        <v>125842.159771438</v>
+      </c>
+      <c r="T74" s="5">
+        <v>172164.54791011399</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C75" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75">
+        <v>3.9</v>
+      </c>
+      <c r="F75" s="2">
+        <f t="shared" si="4"/>
+        <v>43856</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="I75" s="2">
+        <v>43901</v>
+      </c>
+      <c r="K75" s="5">
+        <v>4644718.6398688396</v>
+      </c>
+      <c r="L75" s="5">
+        <v>1691688.4168060001</v>
+      </c>
+      <c r="M75" s="5">
+        <v>3177073.4424424502</v>
+      </c>
+      <c r="N75" s="5">
+        <v>68425.625609726398</v>
+      </c>
+      <c r="O75" s="5">
+        <v>102.443947741521</v>
+      </c>
+      <c r="P75" s="5">
+        <v>583.59997432904902</v>
+      </c>
+      <c r="Q75" s="5">
+        <v>1377.6501074088701</v>
+      </c>
+      <c r="R75" s="5">
+        <v>5809.40057932735</v>
+      </c>
+      <c r="S75" s="5">
+        <v>29715.434521759798</v>
+      </c>
+      <c r="T75" s="5">
+        <v>30837.096479159802</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" s="2">
+        <v>43861</v>
+      </c>
+      <c r="C76" s="2">
+        <v>43895</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76">
+        <v>3.9</v>
+      </c>
+      <c r="F76" s="2">
+        <f t="shared" si="4"/>
+        <v>43850</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="I76" s="2">
+        <v>43895</v>
+      </c>
+      <c r="K76" s="5">
+        <v>32247215.2647692</v>
+      </c>
+      <c r="L76" s="5">
+        <v>11203461.579791799</v>
+      </c>
+      <c r="M76" s="5">
+        <v>21040647.368829101</v>
+      </c>
+      <c r="N76" s="5">
+        <v>453159.14279132901</v>
+      </c>
+      <c r="O76" s="5">
+        <v>886.97096380056303</v>
+      </c>
+      <c r="P76" s="5">
+        <v>3977.1449308568399</v>
+      </c>
+      <c r="Q76" s="5">
+        <v>9759.0941135325393</v>
+      </c>
+      <c r="R76" s="5">
+        <v>40406.751804524101</v>
+      </c>
+      <c r="S76" s="5">
+        <v>191217.52320610301</v>
+      </c>
+      <c r="T76" s="5">
+        <v>206911.657772512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>